<commit_message>
[feat]: finished invoice document
</commit_message>
<xml_diff>
--- a/src/document-templates/xansha/invoice.xlsx
+++ b/src/document-templates/xansha/invoice.xlsx
@@ -9,16 +9,16 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="l8zTm1Z4ePeegy7NBa2qo3K9AuVkGD9as+JOtl7gan0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="tJxQhKqvcFt6Basl5/9qqaHIECg78LYaMf10tcycsMs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
-    <t>Счет-фактура  {{enumeration}}   от  10  Сентября  2025г.</t>
+    <t>Счет-фактура  {{enumeration}}   от  {{documentDateTo}}.</t>
   </si>
   <si>
     <t>Поставщик: Индивидуальны  предприниматель " XANSHA"  Рыспаева Гаухар Сериковна</t>
@@ -52,7 +52,7 @@
     <t>Договор (контракт) на поставку товаров (работ, услуг):без  договора</t>
   </si>
   <si>
-    <t>Условия оплаты по договору (контракту): наличный расчет №0451    от   09.09.2025гг</t>
+    <t>Условия оплаты по договору (контракту): наличный расчет {{enumeration}}  от   {{documentDateFrom}}</t>
   </si>
   <si>
     <t xml:space="preserve">Пункт назначения поставляемых товаров (работ, услуг): </t>
@@ -95,33 +95,7 @@
     <t>(ИИН, наименование и адрес)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>Грузополучатель: ТОО  "Оптиктелеком СтройСервис"</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>РК, 050010, г.Алматы</t>
-    </r>
+    <t>Грузополучатель: {{organization}}, {{city}}</t>
   </si>
   <si>
     <r>
@@ -139,7 +113,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> БИН:041240005176, РК, г.Алматы, ул. Кармысова К, д.76/2                   </t>
+      <t xml:space="preserve"> БИН:{{bin}}, РК, {{city}}, {{address}}                   </t>
     </r>
   </si>
   <si>
@@ -150,7 +124,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> ИИК грузополучателя: </t>
+      <t xml:space="preserve">ИИК грузополучателя: </t>
     </r>
     <r>
       <rPr>
@@ -159,30 +133,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> KZ338562203117660575 (KZТ), в банке АО "БанкЦентрКредит" г.Астана, БИК:KCJBKZKX  </t>
-    </r>
-  </si>
-  <si>
-    <t>Свидетельство НДС: серия 60001 №0037936 от 13.08.2012г, Код 17, ОКЭД 42.22.0, ОКПО:40413189</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve"> Генеральный директор: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>Жигулин Олег Александрович, действующий на основании Устава</t>
+      <t xml:space="preserve"> {{iik}} (KZТ), в банке {{bank}} {{city}}, БИК:{{bik}} </t>
     </r>
   </si>
   <si>
@@ -219,10 +170,16 @@
     <t>Сумма</t>
   </si>
   <si>
-    <t>За проживание                     Адильбеков Ж.Е.                             с 09.09.2025г - 10.09.2025г</t>
+    <t>Проживание:                     {{fullnameClient}}                             с {{documentDateFromNumeric}} - {{documentDateToNumeric}}</t>
   </si>
   <si>
     <t>сут</t>
+  </si>
+  <si>
+    <t>{{perAmount}},00</t>
+  </si>
+  <si>
+    <t>{{totalAmount}},00</t>
   </si>
   <si>
     <t>без НДС</t>
@@ -231,7 +188,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Всего по счету: Двадцать тысячи  тенге 00 тиын</t>
+    <t>Всего по счету: {{totalAmountRussian}} тенге 00 тиын</t>
   </si>
   <si>
     <t>Руководитель: Рыспаева Г.С.</t>
@@ -546,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -580,6 +537,9 @@
     </xf>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -596,15 +556,12 @@
     </xf>
     <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -654,22 +611,28 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="23" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -709,7 +672,7 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="342900" cy="57150"/>
@@ -767,7 +730,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="352425" cy="552450"/>
@@ -1038,14 +1001,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="16.83" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.33"/>
-    <col customWidth="1" min="2" max="2" width="26.5"/>
+    <col customWidth="1" min="2" max="2" width="22.0"/>
     <col customWidth="1" min="3" max="3" width="14.0"/>
     <col customWidth="1" min="4" max="4" width="12.83"/>
     <col customWidth="1" min="5" max="5" width="19.67"/>
-    <col customWidth="1" min="6" max="6" width="13.83"/>
+    <col customWidth="1" min="6" max="6" width="14.83"/>
     <col customWidth="1" min="7" max="7" width="8.83"/>
     <col customWidth="1" min="8" max="8" width="9.17"/>
-    <col customWidth="1" min="9" max="9" width="12.17"/>
+    <col customWidth="1" min="9" max="9" width="14.67"/>
     <col customWidth="1" min="10" max="10" width="10.17"/>
     <col customWidth="1" min="11" max="11" width="11.33"/>
     <col customWidth="1" min="12" max="26" width="8.0"/>
@@ -1164,7 +1127,7 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" ht="11.25" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="13"/>
@@ -1179,25 +1142,25 @@
       <c r="K11" s="14"/>
     </row>
     <row r="12" ht="11.25" customHeight="1">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" ht="11.25" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" ht="11.25" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -1245,13 +1208,13 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" ht="11.25" customHeight="1">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" ht="11.25" customHeight="1">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="9"/>
@@ -1263,25 +1226,25 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" ht="11.25" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" ht="11.25" customHeight="1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="9"/>
@@ -1293,25 +1256,25 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="21"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" ht="11.25" customHeight="1">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="24"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="25"/>
     </row>
     <row r="22" ht="11.25" customHeight="1">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
@@ -1323,288 +1286,284 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="21"/>
-    </row>
-    <row r="23" ht="11.25" customHeight="1">
-      <c r="A23" s="20" t="s">
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" ht="9.75" customHeight="1">
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" ht="11.25" customHeight="1">
+      <c r="A24" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="21"/>
-    </row>
-    <row r="24" ht="11.25" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="B24" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="21"/>
-    </row>
-    <row r="25" ht="9.75" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="28"/>
-    </row>
-    <row r="26" ht="11.25" customHeight="1">
-      <c r="A26" s="29" t="s">
+      <c r="C24" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="D24" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="E24" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="F24" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="G24" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="H24" s="22"/>
+      <c r="I24" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="J24" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="30" t="s">
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" ht="34.5" customHeight="1">
+      <c r="A25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="H25" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="K26" s="10"/>
-    </row>
-    <row r="27" ht="34.5" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36" t="s">
+      <c r="I25" s="34"/>
+      <c r="J25" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" ht="9.75" customHeight="1">
+      <c r="A26" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="B26" s="40">
+        <v>2.0</v>
+      </c>
+      <c r="C26" s="40">
+        <v>3.0</v>
+      </c>
+      <c r="D26" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="40">
+        <v>5.0</v>
+      </c>
+      <c r="F26" s="41">
+        <v>6.0</v>
+      </c>
+      <c r="G26" s="40">
+        <v>7.0</v>
+      </c>
+      <c r="H26" s="40">
+        <v>8.0</v>
+      </c>
+      <c r="I26" s="40">
+        <v>9.0</v>
+      </c>
+      <c r="J26" s="40">
+        <v>10.0</v>
+      </c>
+      <c r="K26" s="42">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="27" ht="55.5" customHeight="1">
+      <c r="A27" s="43">
+        <v>1.0</v>
+      </c>
+      <c r="B27" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="C27" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" ht="9.75" customHeight="1">
-      <c r="A28" s="39">
+      <c r="D27" s="45">
         <v>1.0</v>
       </c>
-      <c r="B28" s="40">
-        <v>2.0</v>
-      </c>
-      <c r="C28" s="40">
-        <v>3.0</v>
-      </c>
-      <c r="D28" s="40">
-        <v>4.0</v>
-      </c>
-      <c r="E28" s="40">
-        <v>5.0</v>
-      </c>
-      <c r="F28" s="41">
-        <v>6.0</v>
-      </c>
-      <c r="G28" s="40">
-        <v>7.0</v>
-      </c>
-      <c r="H28" s="40">
-        <v>8.0</v>
-      </c>
-      <c r="I28" s="40">
-        <v>9.0</v>
-      </c>
-      <c r="J28" s="40">
-        <v>10.0</v>
-      </c>
-      <c r="K28" s="42">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="29" ht="55.5" customHeight="1">
-      <c r="A29" s="43">
-        <v>1.0</v>
-      </c>
-      <c r="B29" s="44" t="s">
+      <c r="E27" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="F27" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="45">
-        <v>1.0</v>
-      </c>
-      <c r="E29" s="46">
-        <v>20000.0</v>
-      </c>
-      <c r="F29" s="46">
-        <v>20000.0</v>
-      </c>
-      <c r="G29" s="47" t="s">
+      <c r="G27" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46">
-        <v>20000.0</v>
+      <c r="H27" s="48"/>
+      <c r="I27" s="46" t="s">
+        <v>32</v>
       </c>
-      <c r="J29" s="45" t="s">
+      <c r="J27" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="48"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="49" t="s">
+      <c r="K27" s="49"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="50">
-        <v>20000.0</v>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="51" t="s">
+        <v>32</v>
       </c>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50">
-        <v>20000.0</v>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="51" t="s">
+        <v>32</v>
       </c>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-    </row>
-    <row r="31" ht="9.75" customHeight="1">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+    </row>
+    <row r="29" ht="9.75" customHeight="1">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" ht="11.25" customHeight="1">
+      <c r="A30" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+    </row>
+    <row r="31" ht="31.5" customHeight="1">
+      <c r="A31" s="56"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" ht="11.25" customHeight="1">
-      <c r="A32" s="52" t="s">
-        <v>36</v>
+      <c r="A32" s="59" t="s">
+        <v>38</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
-      <c r="H32" s="53" t="s">
-        <v>37</v>
+      <c r="H32" s="59" t="s">
+        <v>39</v>
       </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-    </row>
-    <row r="33" ht="31.5" customHeight="1">
-      <c r="A33" s="54"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
+    </row>
+    <row r="33" ht="11.25" customHeight="1">
+      <c r="A33" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
     </row>
     <row r="34" ht="11.25" customHeight="1">
-      <c r="A34" s="57" t="s">
-        <v>38</v>
-      </c>
+      <c r="A34" s="56"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
-      <c r="H34" s="57" t="s">
-        <v>39</v>
-      </c>
+      <c r="H34" s="56"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
     </row>
     <row r="35" ht="11.25" customHeight="1">
-      <c r="A35" s="52" t="s">
-        <v>40</v>
+      <c r="A35" s="59" t="s">
+        <v>38</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="H35" s="59" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" ht="11.25" customHeight="1">
-      <c r="A36" s="54"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
     </row>
     <row r="37" ht="11.25" customHeight="1">
-      <c r="A37" s="57" t="s">
-        <v>38</v>
+      <c r="A37" s="27" t="s">
+        <v>41</v>
       </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="57" t="s">
-        <v>38</v>
-      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38" ht="11.25" customHeight="1">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-    </row>
-    <row r="39" ht="11.25" customHeight="1">
-      <c r="A39" s="27" t="s">
-        <v>41</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" ht="9.75" customHeight="1">
+      <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
@@ -1616,18 +1575,18 @@
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
     </row>
-    <row r="40" ht="11.25" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+    <row r="40" ht="9.75" customHeight="1">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
     </row>
     <row r="41" ht="9.75" customHeight="1">
       <c r="A41" s="27"/>
@@ -14083,34 +14042,8 @@
       <c r="J998" s="27"/>
       <c r="K998" s="27"/>
     </row>
-    <row r="999" ht="9.75" customHeight="1">
-      <c r="A999" s="27"/>
-      <c r="B999" s="27"/>
-      <c r="C999" s="27"/>
-      <c r="D999" s="27"/>
-      <c r="E999" s="27"/>
-      <c r="F999" s="27"/>
-      <c r="G999" s="27"/>
-      <c r="H999" s="27"/>
-      <c r="I999" s="27"/>
-      <c r="J999" s="27"/>
-      <c r="K999" s="27"/>
-    </row>
-    <row r="1000" ht="9.75" customHeight="1">
-      <c r="A1000" s="27"/>
-      <c r="B1000" s="27"/>
-      <c r="C1000" s="27"/>
-      <c r="D1000" s="27"/>
-      <c r="E1000" s="27"/>
-      <c r="F1000" s="27"/>
-      <c r="G1000" s="27"/>
-      <c r="H1000" s="27"/>
-      <c r="I1000" s="27"/>
-      <c r="J1000" s="27"/>
-      <c r="K1000" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="39">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A6:K6"/>
@@ -14130,28 +14063,26 @@
     <mergeCell ref="A20:K20"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="I24:I25"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="A35:E35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="A33:E33"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
[feat]: made ui for dynamic rows for invoice document
</commit_message>
<xml_diff>
--- a/src/document-templates/xansha/invoice.xlsx
+++ b/src/document-templates/xansha/invoice.xlsx
@@ -95,7 +95,24 @@
     <t>(ИИН, наименование и адрес)</t>
   </si>
   <si>
-    <t>Грузополучатель: {{organization}}, {{city}}</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Грузополучатель: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>{{organization}}, {{city}}</t>
+    </r>
   </si>
   <si>
     <r>
@@ -133,7 +150,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> {{iik}} (KZТ), в банке {{bank}} {{city}}, БИК:{{bik}} </t>
+      <t xml:space="preserve"> {{iik}} (KZТ), в банке {{bank}} {{city}}, БИК:{{bik}}</t>
     </r>
   </si>
   <si>
@@ -14058,30 +14075,30 @@
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A16:K16"/>
     <mergeCell ref="A17:K17"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A20:K20"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A22:K22"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="J24:K24"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:E35"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="H35:K35"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A31:E31"/>
-    <mergeCell ref="H31:K31"/>
     <mergeCell ref="A32:E32"/>
-    <mergeCell ref="H32:K32"/>
     <mergeCell ref="A33:E33"/>
   </mergeCells>
   <printOptions/>

</xml_diff>